<commit_message>
puma level analysis under 45
</commit_message>
<xml_diff>
--- a/data/co_missing_hh.xlsx
+++ b/data/co_missing_hh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\SDO Housing\shortfall\statewide_total_shortfall_estimates\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5FC4387-9554-4F50-AC30-A1607BAA5406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0B3B5A-7835-477E-B398-6E71EE49F5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7116" yWindow="0" windowWidth="30960" windowHeight="12120" xr2:uid="{93AA90D6-C3BD-4DAD-A718-360AC19A9E3D}"/>
   </bookViews>
@@ -16,15 +16,39 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="co_missing_hh" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="Slicer_variable">#N/A</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId4"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="17">
   <si>
     <t>baseline_year</t>
   </si>
@@ -81,6 +105,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,7 +542,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -557,16 +585,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -606,11 +636,109 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="32">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -621,6 +749,2399 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[co_missing_hh.xlsx]Sheet1!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>current_hh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1656640</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1759996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1777348</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1800546</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1837352</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1852775</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1849895</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1861196</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1898642</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1910173</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1960642</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1975400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1996107</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2002731</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2039600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2074731</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2109050</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2139167</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2176768</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2235163</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2205583</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2313012</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2384564</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2428261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2AE-4765-AF51-B50058D4FB7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$4:$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>households</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1658043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1753854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1804111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1821318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1850238</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1812944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1846980</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1859961</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1897840</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1910144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1960583</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1975398</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1996089</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2002794</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2039591</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2074739</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2108996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2139204</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2176758</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2235119</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2205583</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2313036</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2384579</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2428263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CC1-4937-9BE8-5FEA9DDDCC10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$4:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>missing_hh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>90228.176686954699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69224.051835865394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78805.988748624804</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80231.159687489795</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91000.817717514801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87575.333921278594</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112945.52843789601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92440.904794975897</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91809.408034207998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103372.28899519501</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>106809.469351441</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>115649.1729755</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>119376.839363882</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100314.317752009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85747.490034989896</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91594.037249839603</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>84676.153345970306</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92215.8022770596</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>92919.239178487696</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104861.263603306</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90577.791187163893</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>92396.145443414804</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>102434.42815049599</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>87786.265729248495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CC1-4937-9BE8-5FEA9DDDCC10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$4:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>target_hh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1746868.17668695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1829220.0518358599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1856153.98874862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1880777.15968749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1928352.81771751</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1940350.33392127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1962840.5284378901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1953636.9047949701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1990451.4080342001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013545.2889951901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2067451.46935144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2091049.1729755001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2115483.83936388</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2103045.3177519999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2125347.49003499</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2166325.0372498399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2193726.15334597</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2231382.80227705</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2269687.2391784801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2340024.2636032999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2296160.7911871602</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2405408.1454434101</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2486998.4281504899</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2516047.2657292401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4CC1-4937-9BE8-5FEA9DDDCC10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$4:$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>underproduction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>107055.449144162</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79046.528248279501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83392.882893289396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51819.694407884199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66700.281807910593</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38561.667285556403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63667.503618838702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24430.8997841852</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40741.797930745401</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55656.830521258496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68362.599317306594</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84347.287342632102</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>103398.146698824</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81786.229212641701</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70171.410563147598</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85633.5655261473</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85883.582469442801</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87640.949765325902</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>85508.935977355504</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>112299.119582427</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>104768.35914438299</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>107172.83730885699</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>125772.871737364</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>112680.911293945</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4CC1-4937-9BE8-5FEA9DDDCC10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2117744271"/>
+        <c:axId val="2117738031"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2117744271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117738031"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2117738031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2117744271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D300C978-3BF3-F748-FC2A-07F2E08AB578}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13335</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="variable">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05DBBB19-85DC-2A8E-2E4B-94C9B65E4A3B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="variable"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8473440" y="2186940"/>
+              <a:ext cx="1828800" cy="2581275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,7 +3202,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1334840057"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -1989,8 +4510,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6C80C3E6-1667-4D68-A298-60C6FEA39E3D}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:K30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6C80C3E6-1667-4D68-A298-60C6FEA39E3D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A4:G30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField axis="axisPage" showAll="0">
       <items count="2">
@@ -2031,13 +4552,13 @@
       <items count="10">
         <item x="1"/>
         <item x="3"/>
-        <item x="5"/>
+        <item h="1" x="5"/>
         <item x="2"/>
-        <item x="6"/>
+        <item h="1" x="6"/>
         <item x="0"/>
         <item x="8"/>
-        <item x="7"/>
-        <item x="4"/>
+        <item h="1" x="7"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2126,7 +4647,7 @@
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="10">
+  <colItems count="6">
     <i>
       <x/>
     </i>
@@ -2134,25 +4655,13 @@
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
-    </i>
-    <i>
       <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
     </i>
     <i>
       <x v="5"/>
     </i>
     <i>
       <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -2162,8 +4671,130 @@
     <pageField fld="0" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of value" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of value" fld="3" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
+  <formats count="2">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="9">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2174,6 +4805,35 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_variable" xr10:uid="{166A344A-E60B-489E-91E0-06BEF49E8133}" sourceName="variable">
+  <pivotTables>
+    <pivotTable tabId="2" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1334840057">
+      <items count="9">
+        <i x="1" s="1"/>
+        <i x="3" s="1"/>
+        <i x="5"/>
+        <i x="2" s="1"/>
+        <i x="6"/>
+        <i x="0" s="1"/>
+        <i x="8" s="1"/>
+        <i x="7"/>
+        <i x="4"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="variable" xr10:uid="{4227A929-2C37-41B2-8971-1281D27F0753}" cache="Slicer_variable" caption="variable" startItem="2" rowHeight="247650"/>
+</slicers>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2493,36 +5153,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EF390B-84DC-4B28-AAF2-32E54ECCF62D}">
-  <dimension ref="A2:K30"/>
+  <dimension ref="A2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2530,7 +5190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2541,907 +5201,795 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B6" s="3">
         <v>1656640</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1658043</v>
       </c>
-      <c r="D6" s="2">
-        <v>1807842</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="3">
         <v>90228.176686954699</v>
       </c>
-      <c r="F6" s="2">
-        <v>74612</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="E6" s="3">
         <v>1746868.17668695</v>
       </c>
-      <c r="H6" s="2">
+      <c r="F6" s="3">
         <v>107055.449144162</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K6" s="2">
-        <v>7141288.8525180668</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="G6" s="3">
+        <v>5258834.802518067</v>
+      </c>
+      <c r="H6" s="3">
+        <f>F6-D6</f>
+        <v>16827.272457207306</v>
+      </c>
+      <c r="I6" s="4">
+        <f>H6/E6</f>
+        <v>9.6328232901473597E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>2001</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>1759996</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>1753854</v>
       </c>
-      <c r="D7" s="2">
-        <v>1874400</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="3">
         <v>69224.051835865394</v>
       </c>
-      <c r="F7" s="2">
-        <v>34417</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="E7" s="3">
         <v>1829220.0518358599</v>
       </c>
-      <c r="H7" s="2">
+      <c r="F7" s="3">
         <v>79046.528248279501</v>
       </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K7" s="2">
-        <v>7400157.681920005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="G7" s="3">
+        <v>5491340.6319200043</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" ref="H7:H29" si="0">F7-D7</f>
+        <v>9822.4764124141075</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:I29" si="1">H7/E7</f>
+        <v>5.3697620483418472E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>2002</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>1777348</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>1804111</v>
       </c>
-      <c r="D8" s="2">
-        <v>1929092</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="3">
         <v>78805.988748624804</v>
       </c>
-      <c r="F8" s="2">
-        <v>30467</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="E8" s="3">
         <v>1856153.98874862</v>
       </c>
-      <c r="H8" s="2">
+      <c r="F8" s="3">
         <v>83392.882893289396</v>
       </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K8" s="2">
-        <v>7559370.9103905344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="G8" s="3">
+        <v>5599811.8603905346</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>4586.8941446645913</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>2.4711819021852703E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>2003</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>1800546</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>1821318</v>
       </c>
-      <c r="D9" s="2">
-        <v>1973622</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="3">
         <v>80231.159687489795</v>
       </c>
-      <c r="F9" s="2">
-        <v>23811</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="E9" s="3">
         <v>1880777.15968749</v>
       </c>
-      <c r="H9" s="2">
+      <c r="F9" s="3">
         <v>51819.694407884199</v>
       </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K9" s="2">
-        <v>7632125.0637828643</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="G9" s="3">
+        <v>5634692.0137828635</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>-28411.465279605596</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.5106236873020325E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>2004</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>1837352</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1850238</v>
       </c>
-      <c r="D10" s="2">
-        <v>2010806</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="3">
         <v>91000.817717514801</v>
       </c>
-      <c r="F10" s="2">
-        <v>34097</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="E10" s="3">
         <v>1928352.81771751</v>
       </c>
-      <c r="H10" s="2">
+      <c r="F10" s="3">
         <v>66700.281807910593</v>
       </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K10" s="2">
-        <v>7818546.9672429357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="G10" s="3">
+        <v>5773643.9172429359</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>-24300.535909604208</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.2601706330051922E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>2005</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>1852775</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>1812944</v>
       </c>
-      <c r="D11" s="2">
-        <v>2046678</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D11" s="3">
         <v>87575.333921278594</v>
       </c>
-      <c r="F11" s="2">
-        <v>84693</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="E11" s="3">
         <v>1940350.33392127</v>
       </c>
-      <c r="H11" s="2">
+      <c r="F11" s="3">
         <v>38561.667285556403</v>
       </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K11" s="2">
-        <v>7863577.3851281041</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="G11" s="3">
+        <v>5732206.3351281043</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>-49013.666635722191</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.5260215013167272E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>2006</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>1849895</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>1846980</v>
       </c>
-      <c r="D12" s="2">
-        <v>2095235</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="3">
         <v>112945.52843789601</v>
       </c>
-      <c r="F12" s="2">
-        <v>95823</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="E12" s="3">
         <v>1962840.5284378901</v>
       </c>
-      <c r="H12" s="2">
+      <c r="F12" s="3">
         <v>63667.503618838702</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K12" s="2">
-        <v>8027386.6104946239</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="G12" s="3">
+        <v>5836328.5604946241</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>-49278.024819057304</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.5105465321869424E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>2007</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>1861196</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>1859961</v>
       </c>
-      <c r="D13" s="2">
-        <v>2127358</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="3">
         <v>92440.904794975897</v>
       </c>
-      <c r="F13" s="2">
-        <v>96629</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="E13" s="3">
         <v>1953636.9047949701</v>
       </c>
-      <c r="H13" s="2">
+      <c r="F13" s="3">
         <v>24430.8997841852</v>
       </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K13" s="2">
-        <v>8015652.7593741314</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="G13" s="3">
+        <v>5791665.7093741316</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>-68010.005010790701</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.4811998505898514E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>2008</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>1898642</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>1897840</v>
       </c>
-      <c r="D14" s="2">
-        <v>2152124</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="3">
         <v>91809.408034207998</v>
       </c>
-      <c r="F14" s="2">
-        <v>98498</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="E14" s="3">
         <v>1990451.4080342001</v>
       </c>
-      <c r="H14" s="2">
+      <c r="F14" s="3">
         <v>40741.797930745401</v>
       </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K14" s="2">
-        <v>8170106.6639991533</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="G14" s="3">
+        <v>5919484.6139991535</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>-51067.610103462597</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.5656295801713514E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>2009</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>1910173</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>1910144</v>
       </c>
-      <c r="D15" s="2">
-        <v>2167902</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="D15" s="3">
         <v>103372.28899519501</v>
       </c>
-      <c r="F15" s="2">
-        <v>104068</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="E15" s="3">
         <v>2013545.2889951901</v>
       </c>
-      <c r="H15" s="2">
+      <c r="F15" s="3">
         <v>55656.830521258496</v>
       </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K15" s="2">
-        <v>8264861.4585116431</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="G15" s="3">
+        <v>5992891.4085116433</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>-47715.458473936509</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.3697236280067844E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>2010</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>1960642</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>1960583</v>
       </c>
-      <c r="D16" s="2">
-        <v>2214262</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="3">
         <v>106809.469351441</v>
       </c>
-      <c r="F16" s="2">
-        <v>106422</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="E16" s="3">
         <v>2067451.46935144</v>
       </c>
-      <c r="H16" s="2">
+      <c r="F16" s="3">
         <v>68362.599317306594</v>
       </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K16" s="2">
-        <v>8484532.5880201887</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="G16" s="3">
+        <v>6163848.538020188</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>-38446.870034134408</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.8596262405228405E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>2011</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>1975400</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>1975398</v>
       </c>
-      <c r="D17" s="2">
-        <v>2224661</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="3">
         <v>115649.1729755</v>
       </c>
-      <c r="F17" s="2">
-        <v>107906</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="E17" s="3">
         <v>2091049.1729755001</v>
       </c>
-      <c r="H17" s="2">
+      <c r="F17" s="3">
         <v>84347.287342632102</v>
       </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K17" s="2">
-        <v>8574410.6832936332</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="G17" s="3">
+        <v>6241843.6332936324</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
+        <v>-31301.885632867896</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.4969464151015757E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>2012</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>1996107</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>1996089</v>
       </c>
-      <c r="D18" s="2">
-        <v>2230536</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D18" s="3">
         <v>119376.839363882</v>
       </c>
-      <c r="F18" s="2">
-        <v>107128</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="E18" s="3">
         <v>2115483.83936388</v>
       </c>
-      <c r="H18" s="2">
+      <c r="F18" s="3">
         <v>103398.146698824</v>
       </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K18" s="2">
-        <v>8668118.8754265867</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="G18" s="3">
+        <v>6330454.825426586</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="0"/>
+        <v>-15978.692665057999</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="1"/>
+        <v>-7.5532095153526425E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>2013</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>2002731</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>2002794</v>
       </c>
-      <c r="D19" s="2">
-        <v>2247291</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="3">
         <v>100314.317752009</v>
       </c>
-      <c r="F19" s="2">
-        <v>115279</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="E19" s="3">
         <v>2103045.3177519999</v>
       </c>
-      <c r="H19" s="2">
+      <c r="F19" s="3">
         <v>81786.229212641701</v>
       </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K19" s="2">
-        <v>8653240.9147166517</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="G19" s="3">
+        <v>6290670.8647166509</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>-18528.088539367294</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="1"/>
+        <v>-8.8101232926223634E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>2014</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>2039600</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>2039591</v>
       </c>
-      <c r="D20" s="2">
-        <v>2276280</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="3">
         <v>85747.490034989896</v>
       </c>
-      <c r="F20" s="2">
-        <v>109253</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="E20" s="3">
         <v>2125347.49003499</v>
       </c>
-      <c r="H20" s="2">
+      <c r="F20" s="3">
         <v>70171.410563147598</v>
       </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K20" s="2">
-        <v>8745990.4406331275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="G20" s="3">
+        <v>6360457.3906331277</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
+        <v>-15576.079471842299</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="1"/>
+        <v>-7.3287213243354698E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>2015</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>2074731</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>2074739</v>
       </c>
-      <c r="D21" s="2">
-        <v>2309122</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="D21" s="3">
         <v>91594.037249839603</v>
       </c>
-      <c r="F21" s="2">
-        <v>114405</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="E21" s="3">
         <v>2166325.0372498399</v>
       </c>
-      <c r="H21" s="2">
+      <c r="F21" s="3">
         <v>85633.5655261473</v>
       </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K21" s="2">
-        <v>8916549.6900258269</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="G21" s="3">
+        <v>6493022.6400258271</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="0"/>
+        <v>-5960.4717236923025</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.7514207799856066E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>2016</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>2109050</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>2108996</v>
       </c>
-      <c r="D22" s="2">
-        <v>2339140</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="D22" s="3">
         <v>84676.153345970306</v>
       </c>
-      <c r="F22" s="2">
-        <v>115895</v>
-      </c>
-      <c r="G22" s="2">
+      <c r="E22" s="3">
         <v>2193726.15334597</v>
       </c>
-      <c r="H22" s="2">
+      <c r="F22" s="3">
         <v>85883.582469442801</v>
       </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K22" s="2">
-        <v>9037366.9391613845</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="G22" s="3">
+        <v>6582331.8891613837</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="0"/>
+        <v>1207.4291234724951</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5040102504629843E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>2017</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="3">
         <v>2139167</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>2139204</v>
       </c>
-      <c r="D23" s="2">
-        <v>2385495</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="3">
         <v>92215.8022770596</v>
       </c>
-      <c r="F23" s="2">
-        <v>124273</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="E23" s="3">
         <v>2231382.80227705</v>
       </c>
-      <c r="H23" s="2">
+      <c r="F23" s="3">
         <v>87640.949765325902</v>
       </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K23" s="2">
-        <v>9199378.6043194365</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="G23" s="3">
+        <v>6689610.5543194348</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="0"/>
+        <v>-4574.8525117336976</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.0502320386556788E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>2018</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>2176768</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>2176758</v>
       </c>
-      <c r="D24" s="2">
-        <v>2424128</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="3">
         <v>92919.239178487696</v>
       </c>
-      <c r="F24" s="2">
-        <v>120503</v>
-      </c>
-      <c r="G24" s="2">
+      <c r="E24" s="3">
         <v>2269687.2391784801</v>
       </c>
-      <c r="H24" s="2">
+      <c r="F24" s="3">
         <v>85508.935977355504</v>
       </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K24" s="2">
-        <v>9346272.464334324</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="G24" s="3">
+        <v>6801641.4143343242</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="0"/>
+        <v>-7410.303201132192</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.2649005877190256E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>2019</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>2235163</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>2235119</v>
       </c>
-      <c r="D25" s="2">
-        <v>2464109</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="3">
         <v>104861.263603306</v>
       </c>
-      <c r="F25" s="2">
-        <v>113271</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="E25" s="3">
         <v>2340024.2636032999</v>
       </c>
-      <c r="H25" s="2">
+      <c r="F25" s="3">
         <v>112299.119582427</v>
       </c>
-      <c r="I25" s="2">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K25" s="2">
-        <v>9604846.6967890356</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="G25" s="3">
+        <v>7027466.646789033</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="0"/>
+        <v>7437.8559791209991</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="1"/>
+        <v>3.1785379727933992E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>2020</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="3">
         <v>2205583</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>2205583</v>
       </c>
-      <c r="D26" s="2">
-        <v>2437665</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="3">
         <v>90577.791187163893</v>
       </c>
-      <c r="F26" s="2">
-        <v>113422</v>
-      </c>
-      <c r="G26" s="2">
+      <c r="E26" s="3">
         <v>2296160.7911871602</v>
       </c>
-      <c r="H26" s="2">
+      <c r="F26" s="3">
         <v>104768.35914438299</v>
       </c>
-      <c r="I26" s="2">
-        <v>12000</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K26" s="2">
-        <v>9465759.9915187061</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="G26" s="3">
+        <v>6902672.9415187063</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" si="0"/>
+        <v>14190.5679572191</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" si="1"/>
+        <v>6.1801281563920001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>2021</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>2313012</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>2313036</v>
       </c>
-      <c r="D27" s="2">
-        <v>2540783</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="D27" s="3">
         <v>92396.145443414804</v>
       </c>
-      <c r="F27" s="2">
-        <v>103232</v>
-      </c>
-      <c r="G27" s="2">
+      <c r="E27" s="3">
         <v>2405408.1454434101</v>
       </c>
-      <c r="H27" s="2">
+      <c r="F27" s="3">
         <v>107172.83730885699</v>
       </c>
-      <c r="I27" s="2">
-        <v>12690</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K27" s="2">
-        <v>9887730.1781956833</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="G27" s="3">
+        <v>7231025.1281956816</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" si="0"/>
+        <v>14776.69186544219</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="1"/>
+        <v>6.1431120924047055E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>2022</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="3">
         <v>2384564</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <v>2384579</v>
       </c>
-      <c r="D28" s="2">
-        <v>2590205</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="D28" s="3">
         <v>102434.42815049599</v>
       </c>
-      <c r="F28" s="2">
-        <v>90097</v>
-      </c>
-      <c r="G28" s="2">
+      <c r="E28" s="3">
         <v>2486998.4281504899</v>
       </c>
-      <c r="H28" s="2">
+      <c r="F28" s="3">
         <v>125772.871737364</v>
       </c>
-      <c r="I28" s="2">
-        <v>7972</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K28" s="2">
-        <v>10172622.778038353</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="G28" s="3">
+        <v>7484348.7280383501</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="0"/>
+        <v>23338.443586868001</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="1"/>
+        <v>9.3841810765534495E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>2023</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="3">
         <v>2428261</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>2428263</v>
       </c>
-      <c r="D29" s="2">
-        <v>2638093</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="3">
         <v>87786.265729248495</v>
       </c>
-      <c r="F29" s="2">
-        <v>94822</v>
-      </c>
-      <c r="G29" s="2">
+      <c r="E29" s="3">
         <v>2516047.2657292401</v>
       </c>
-      <c r="H29" s="2">
+      <c r="F29" s="3">
         <v>112680.911293945</v>
       </c>
-      <c r="I29" s="2">
-        <v>7479</v>
-      </c>
-      <c r="J29" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="K29" s="2">
-        <v>10313432.492752435</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="G29" s="3">
+        <v>7573038.4427524339</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="0"/>
+        <v>24894.645564696504</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="1"/>
+        <v>9.8943473375016858E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="3">
         <v>48245342</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <v>48256165</v>
       </c>
-      <c r="D30" s="2">
-        <v>53506829</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="D30" s="3">
         <v>2264992.0745028113</v>
       </c>
-      <c r="F30" s="2">
-        <v>2213023</v>
-      </c>
-      <c r="G30" s="2">
+      <c r="E30" s="3">
         <v>50510334.074502707</v>
       </c>
-      <c r="H30" s="2">
+      <c r="F30" s="3">
         <v>1926500.3415819097</v>
       </c>
-      <c r="I30" s="2">
-        <v>40141</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1.2000000000000004</v>
-      </c>
-      <c r="K30" s="2">
-        <v>206963327.69058737</v>
+      <c r="G30" s="3">
+        <v>151203333.49058738</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>